<commit_message>
Grote update voor Alles
Grote update aan:
- Core (70% af)
- Hofposities
- Hoftitels
- Titels
- Encyclopedie

Veel vertalingen zijn nog WIP
</commit_message>
<xml_diff>
--- a/DLP woordenlijst.xlsx
+++ b/DLP woordenlijst.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanp\Documents\Paradox Interactive\Crusader Kings III\mod\DLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16054C38-3722-4524-9FBC-1B511D89BA0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E68BEE7-78BA-4A6F-86C0-7721B939ADD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>Engelse term</t>
   </si>
@@ -167,6 +167,63 @@
   </si>
   <si>
     <t>Complotten</t>
+  </si>
+  <si>
+    <t>Stewardship</t>
+  </si>
+  <si>
+    <t>Rentmeesterschap</t>
+  </si>
+  <si>
+    <t>Diplomacy</t>
+  </si>
+  <si>
+    <t>Diplomatie</t>
+  </si>
+  <si>
+    <t>Martial</t>
+  </si>
+  <si>
+    <t>Krijgshaftigheid</t>
+  </si>
+  <si>
+    <t>Intrige</t>
+  </si>
+  <si>
+    <t>Learning</t>
+  </si>
+  <si>
+    <t>Geleerdheid</t>
+  </si>
+  <si>
+    <t>Prowess</t>
+  </si>
+  <si>
+    <t>Dapperheid</t>
+  </si>
+  <si>
+    <t>Dismiss</t>
+  </si>
+  <si>
+    <t>Ontzet</t>
+  </si>
+  <si>
+    <t>Reject</t>
+  </si>
+  <si>
+    <t>Afwijzen</t>
+  </si>
+  <si>
+    <t>Voor Afwijzen zie: Reject</t>
+  </si>
+  <si>
+    <t>Voor Ontzet zie: Dismiss</t>
+  </si>
+  <si>
+    <t>Aptitude</t>
+  </si>
+  <si>
+    <t>Aanleg</t>
   </si>
 </sst>
 </file>
@@ -236,8 +293,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{620CAB14-0AE3-4DC1-ABD7-5524AAC7191E}" name="Tabel1" displayName="Tabel1" ref="A1:C15" totalsRowShown="0">
-  <autoFilter ref="A1:C15" xr:uid="{620CAB14-0AE3-4DC1-ABD7-5524AAC7191E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{620CAB14-0AE3-4DC1-ABD7-5524AAC7191E}" name="Tabel1" displayName="Tabel1" ref="A1:C24" totalsRowShown="0">
+  <autoFilter ref="A1:C24" xr:uid="{620CAB14-0AE3-4DC1-ABD7-5524AAC7191E}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{BEFD245A-2A28-400B-A9E5-FE2EBA62AFD7}" name="Engelse term"/>
     <tableColumn id="2" xr3:uid="{C7771ADF-0301-48C6-AC98-3DC03BE980CB}" name="Nederlandse term"/>
@@ -510,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,6 +709,84 @@
         <v>31</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Van alles en nog wat
Court positions verder uitgewerkt en voornamlijk nog aan de activiteiten tab gewerkt.
</commit_message>
<xml_diff>
--- a/DLP woordenlijst.xlsx
+++ b/DLP woordenlijst.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanp\Documents\Paradox Interactive\Crusader Kings III\mod\DLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F54F8D-29E6-4BD7-BCC6-FDA0C7E92980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5D70F4-49D8-4352-BD6C-E1A5D1037287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
   <si>
     <t>Engelse term</t>
   </si>
@@ -318,6 +318,30 @@
   </si>
   <si>
     <t>Bevelhebber</t>
+  </si>
+  <si>
+    <t>Grant Title</t>
+  </si>
+  <si>
+    <t>Verleen Titel</t>
+  </si>
+  <si>
+    <t>Hire (Court Position)</t>
+  </si>
+  <si>
+    <t>Benoem</t>
+  </si>
+  <si>
+    <t>Lifestyle</t>
+  </si>
+  <si>
+    <t>Levensstijl</t>
+  </si>
+  <si>
+    <t>Education Focus</t>
+  </si>
+  <si>
+    <t>Onderwijzingsfocus</t>
   </si>
 </sst>
 </file>
@@ -387,8 +411,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{620CAB14-0AE3-4DC1-ABD7-5524AAC7191E}" name="Tabel1" displayName="Tabel1" ref="A1:C37" totalsRowShown="0">
-  <autoFilter ref="A1:C37" xr:uid="{620CAB14-0AE3-4DC1-ABD7-5524AAC7191E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{620CAB14-0AE3-4DC1-ABD7-5524AAC7191E}" name="Tabel1" displayName="Tabel1" ref="A1:C41" totalsRowShown="0">
+  <autoFilter ref="A1:C41" xr:uid="{620CAB14-0AE3-4DC1-ABD7-5524AAC7191E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C32">
     <sortCondition ref="A1:A32"/>
   </sortState>
@@ -664,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,6 +1015,38 @@
         <v>77</v>
       </c>
     </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Edits + Excel bijgewerkt
@tedinnederland kijk eventjes naar wat  van mijn opmerkingen voor de vertalingen in het excel bestand. Ik wil voornamelijk Holding als Heerlijkheden houden, verdere discussies mogelijk natuurlijk ;)
</commit_message>
<xml_diff>
--- a/DLP woordenlijst.xlsx
+++ b/DLP woordenlijst.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanp\Documents\Paradox Interactive\Crusader Kings III\mod\DLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B46377-9C4D-4487-AC81-8CB6548E7D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463E1218-AD2D-4289-8E22-C54146F5BE3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35130" yWindow="2025" windowWidth="16470" windowHeight="16035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="229">
   <si>
     <t>Engelse term</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Levies</t>
-  </si>
-  <si>
-    <t>Baanderheren</t>
   </si>
   <si>
     <r>
@@ -370,9 +367,6 @@
     <t>Marauder</t>
   </si>
   <si>
-    <t>plunderaar</t>
-  </si>
-  <si>
     <t>Milites</t>
   </si>
   <si>
@@ -720,6 +714,76 @@
   </si>
   <si>
     <t>Kanselier</t>
+  </si>
+  <si>
+    <t>Succession</t>
+  </si>
+  <si>
+    <t>Opvolging</t>
+  </si>
+  <si>
+    <t>Succession Law</t>
+  </si>
+  <si>
+    <t>Erfopvolging</t>
+  </si>
+  <si>
+    <t>2024-05-27</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Edit: Ik heb persoonlijk Holding vertaald naar </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Heerlijkheid</t>
+    </r>
+  </si>
+  <si>
+    <t>Kolom1</t>
+  </si>
+  <si>
+    <t>Edit: Zou dit zelf vertalen naar Complotten</t>
+  </si>
+  <si>
+    <t>Edit: Heb ik vertaald naar Broers/Zussen, kan aan de hand van context ook aangepast worden natuurlijk</t>
+  </si>
+  <si>
+    <t>Edit: Vertaald naar Spionnenmeester</t>
+  </si>
+  <si>
+    <t>Raise Levies</t>
+  </si>
+  <si>
+    <t>Baanderheren Oproepen</t>
+  </si>
+  <si>
+    <t>Heervaarders</t>
+  </si>
+  <si>
+    <t>Crusaders</t>
+  </si>
+  <si>
+    <t>Kruisvaarders</t>
+  </si>
+  <si>
+    <t>Edit: Zelf vertaald naar modificatoren</t>
+  </si>
+  <si>
+    <t>Plunderaar</t>
+  </si>
+  <si>
+    <t>Fire (Job)</t>
+  </si>
+  <si>
+    <t>Royeren/Ontslaan</t>
   </si>
 </sst>
 </file>
@@ -797,16 +861,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{620CAB14-0AE3-4DC1-ABD7-5524AAC7191E}" name="Tabel1" displayName="Tabel1" ref="A1:D150" totalsRowShown="0">
-  <autoFilter ref="A1:D150" xr:uid="{620CAB14-0AE3-4DC1-ABD7-5524AAC7191E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{620CAB14-0AE3-4DC1-ABD7-5524AAC7191E}" name="Tabel1" displayName="Tabel1" ref="A1:E150" totalsRowShown="0">
+  <autoFilter ref="A1:E150" xr:uid="{620CAB14-0AE3-4DC1-ABD7-5524AAC7191E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D95">
     <sortCondition ref="A1:A150"/>
   </sortState>
-  <tableColumns count="4">
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{BEFD245A-2A28-400B-A9E5-FE2EBA62AFD7}" name="Engelse term"/>
     <tableColumn id="2" xr3:uid="{C7771ADF-0301-48C6-AC98-3DC03BE980CB}" name="Nederlandse term"/>
     <tableColumn id="3" xr3:uid="{A302C31A-3B76-40AD-A403-4361CBAE6E9E}" name="uitleg"/>
     <tableColumn id="4" xr3:uid="{CBD3F489-A211-4D84-9CF0-2CB3C4563807}" name="Toegevoegd" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{3244FCD1-134B-4EA4-9195-F9ED8CA29B1D}" name="Kolom1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1075,21 +1140,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D95"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="32.42578125" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="68.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1100,62 +1165,65 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+      <c r="E1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
         <v>52</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
         <v>48</v>
       </c>
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
         <v>70</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>71</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>73</v>
       </c>
-      <c r="B6" t="s">
-        <v>74</v>
-      </c>
       <c r="C6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1163,100 +1231,100 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" t="s">
         <v>140</v>
       </c>
-      <c r="B8" t="s">
-        <v>141</v>
-      </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B10" t="s">
+        <v>209</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>200</v>
+      </c>
+      <c r="B13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>210</v>
-      </c>
-      <c r="B10" t="s">
-        <v>211</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>172</v>
-      </c>
-      <c r="B12" t="s">
-        <v>173</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>202</v>
-      </c>
-      <c r="B13" t="s">
-        <v>203</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>144</v>
-      </c>
       <c r="B14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1269,67 +1337,67 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
         <v>26</v>
-      </c>
-      <c r="B19" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
         <v>34</v>
-      </c>
-      <c r="B21" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
         <v>42</v>
       </c>
-      <c r="B22" t="s">
-        <v>43</v>
-      </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
         <v>19</v>
-      </c>
-      <c r="B23" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" t="s">
         <v>62</v>
       </c>
-      <c r="B24" t="s">
-        <v>63</v>
-      </c>
       <c r="C24" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1342,10 +1410,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1358,199 +1426,202 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
         <v>64</v>
       </c>
-      <c r="B28" t="s">
-        <v>65</v>
-      </c>
       <c r="D28" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" t="s">
         <v>77</v>
-      </c>
-      <c r="B29" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B30" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" t="s">
         <v>79</v>
       </c>
-      <c r="B32" t="s">
+      <c r="D32" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>80</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="B33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>81</v>
-      </c>
-      <c r="B33" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>83</v>
-      </c>
-      <c r="B34" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" t="s">
+        <v>131</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>152</v>
+      </c>
+      <c r="B39" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" t="s">
         <v>84</v>
       </c>
-      <c r="C34" t="s">
-        <v>85</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35" t="s">
-        <v>72</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="D40" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>166</v>
+      </c>
+      <c r="B43" t="s">
+        <v>202</v>
+      </c>
+      <c r="C43" t="s">
+        <v>167</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E43" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>203</v>
+      </c>
+      <c r="B44" t="s">
+        <v>204</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>132</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B45" t="s">
         <v>133</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>146</v>
-      </c>
-      <c r="B37" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>88</v>
-      </c>
-      <c r="B38" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>154</v>
-      </c>
-      <c r="B39" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>90</v>
-      </c>
-      <c r="B40" t="s">
-        <v>91</v>
-      </c>
-      <c r="C40" t="s">
-        <v>85</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>92</v>
-      </c>
-      <c r="B41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>148</v>
-      </c>
-      <c r="B42" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>168</v>
-      </c>
-      <c r="B43" t="s">
-        <v>204</v>
-      </c>
-      <c r="C43" t="s">
-        <v>169</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>205</v>
-      </c>
-      <c r="B44" t="s">
-        <v>206</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>134</v>
-      </c>
-      <c r="B45" t="s">
-        <v>135</v>
-      </c>
       <c r="D45" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>29</v>
+      </c>
+      <c r="B46" t="s">
         <v>30</v>
       </c>
-      <c r="B46" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -1558,511 +1629,578 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" t="s">
         <v>17</v>
       </c>
-      <c r="B48" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>197</v>
+      </c>
+      <c r="B49" t="s">
         <v>199</v>
       </c>
-      <c r="B49" t="s">
-        <v>201</v>
-      </c>
       <c r="C49" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D49" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>37</v>
+      </c>
+      <c r="B50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>220</v>
+      </c>
+      <c r="B51" t="s">
+        <v>221</v>
+      </c>
+      <c r="C51" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>172</v>
+      </c>
+      <c r="B52" t="s">
+        <v>173</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>148</v>
+      </c>
+      <c r="B53" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55" t="s">
+        <v>94</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>154</v>
+      </c>
+      <c r="B56" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>95</v>
+      </c>
+      <c r="B57" t="s">
+        <v>96</v>
+      </c>
+      <c r="C57" t="s">
+        <v>84</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>38</v>
-      </c>
-      <c r="B50" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>97</v>
+      </c>
+      <c r="B58" t="s">
+        <v>226</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>35</v>
+      </c>
+      <c r="B59" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>49</v>
+      </c>
+      <c r="B60" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>98</v>
+      </c>
+      <c r="B62" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62" t="s">
+        <v>84</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>191</v>
+      </c>
+      <c r="B63" t="s">
+        <v>193</v>
+      </c>
+      <c r="C63" t="s">
+        <v>192</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E63" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>194</v>
+      </c>
+      <c r="B64" t="s">
+        <v>195</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>100</v>
+      </c>
+      <c r="B65" t="s">
+        <v>100</v>
+      </c>
+      <c r="C65" t="s">
+        <v>101</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>184</v>
+      </c>
+      <c r="B66" t="s">
+        <v>185</v>
+      </c>
+      <c r="C66" t="s">
+        <v>186</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>102</v>
+      </c>
+      <c r="B67" t="s">
+        <v>103</v>
+      </c>
+      <c r="C67" t="s">
+        <v>104</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>169</v>
+      </c>
+      <c r="B69" t="s">
+        <v>168</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>65</v>
+      </c>
+      <c r="B70" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="B71" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>136</v>
+      </c>
+      <c r="B72" t="s">
+        <v>137</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>105</v>
+      </c>
+      <c r="B73" t="s">
+        <v>106</v>
+      </c>
+      <c r="C73" t="s">
+        <v>84</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>43</v>
+      </c>
+      <c r="B74" t="s">
+        <v>44</v>
+      </c>
+      <c r="C74" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>67</v>
+      </c>
+      <c r="B75" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>107</v>
+      </c>
+      <c r="B76" t="s">
+        <v>108</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>109</v>
+      </c>
+      <c r="B77" t="s">
+        <v>110</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>22</v>
+      </c>
+      <c r="B78" t="s">
+        <v>23</v>
+      </c>
+      <c r="C78" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>134</v>
+      </c>
+      <c r="B79" t="s">
+        <v>135</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E79" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>111</v>
+      </c>
+      <c r="B80" t="s">
+        <v>112</v>
+      </c>
+      <c r="C80" t="s">
+        <v>84</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>113</v>
+      </c>
+      <c r="B81" t="s">
+        <v>114</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>187</v>
+      </c>
+      <c r="B82" t="s">
+        <v>188</v>
+      </c>
+      <c r="C82" t="s">
+        <v>189</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E82" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>182</v>
+      </c>
+      <c r="B83" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>54</v>
+      </c>
+      <c r="B84" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>115</v>
+      </c>
+      <c r="B85" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>117</v>
+      </c>
+      <c r="B86" t="s">
+        <v>118</v>
+      </c>
+      <c r="C86" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>206</v>
+      </c>
+      <c r="B87" t="s">
+        <v>207</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E87" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>31</v>
+      </c>
+      <c r="B88" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>58</v>
+      </c>
+      <c r="B89" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>160</v>
+      </c>
+      <c r="B90" t="s">
+        <v>161</v>
+      </c>
+      <c r="C90" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>119</v>
+      </c>
+      <c r="B91" t="s">
+        <v>120</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>121</v>
+      </c>
+      <c r="B92" t="s">
+        <v>122</v>
+      </c>
+      <c r="C92" t="s">
+        <v>123</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>174</v>
+      </c>
+      <c r="B93" t="s">
+        <v>175</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>124</v>
+      </c>
+      <c r="B94" t="s">
+        <v>125</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>126</v>
+      </c>
+      <c r="B95" t="s">
+        <v>127</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>210</v>
+      </c>
+      <c r="B96" t="s">
+        <v>211</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>212</v>
+      </c>
+      <c r="B97" t="s">
+        <v>213</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>12</v>
       </c>
-      <c r="B51" t="s">
-        <v>13</v>
-      </c>
-      <c r="C51" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>174</v>
-      </c>
-      <c r="B52" t="s">
-        <v>175</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>150</v>
-      </c>
-      <c r="B53" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>94</v>
-      </c>
-      <c r="B55" t="s">
-        <v>95</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>156</v>
-      </c>
-      <c r="B56" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>96</v>
-      </c>
-      <c r="B57" t="s">
-        <v>97</v>
-      </c>
-      <c r="C57" t="s">
-        <v>85</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>98</v>
-      </c>
-      <c r="B58" t="s">
-        <v>99</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>36</v>
-      </c>
-      <c r="B59" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>50</v>
-      </c>
-      <c r="B60" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>15</v>
-      </c>
-      <c r="B61" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>100</v>
-      </c>
-      <c r="B62" t="s">
-        <v>101</v>
-      </c>
-      <c r="C62" t="s">
-        <v>85</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>193</v>
-      </c>
-      <c r="B63" t="s">
-        <v>195</v>
-      </c>
-      <c r="C63" t="s">
-        <v>194</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>196</v>
-      </c>
-      <c r="B64" t="s">
-        <v>197</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>102</v>
-      </c>
-      <c r="B65" t="s">
-        <v>102</v>
-      </c>
-      <c r="C65" t="s">
-        <v>103</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>186</v>
-      </c>
-      <c r="B66" t="s">
-        <v>187</v>
-      </c>
-      <c r="C66" t="s">
-        <v>188</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>104</v>
-      </c>
-      <c r="B67" t="s">
-        <v>105</v>
-      </c>
-      <c r="C67" t="s">
-        <v>106</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>21</v>
-      </c>
-      <c r="B68" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>171</v>
-      </c>
-      <c r="B69" t="s">
-        <v>170</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>66</v>
-      </c>
-      <c r="B70" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>40</v>
-      </c>
-      <c r="B71" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>138</v>
-      </c>
-      <c r="B72" t="s">
-        <v>139</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>107</v>
-      </c>
-      <c r="B73" t="s">
-        <v>108</v>
-      </c>
-      <c r="C73" t="s">
-        <v>85</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>44</v>
-      </c>
-      <c r="B74" t="s">
-        <v>45</v>
-      </c>
-      <c r="C74" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>68</v>
-      </c>
-      <c r="B75" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>109</v>
-      </c>
-      <c r="B76" t="s">
-        <v>110</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>111</v>
-      </c>
-      <c r="B77" t="s">
-        <v>112</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>23</v>
-      </c>
-      <c r="B78" t="s">
-        <v>24</v>
-      </c>
-      <c r="C78" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>136</v>
-      </c>
-      <c r="B79" t="s">
-        <v>137</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>113</v>
-      </c>
-      <c r="B80" t="s">
-        <v>114</v>
-      </c>
-      <c r="C80" t="s">
-        <v>85</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>115</v>
-      </c>
-      <c r="B81" t="s">
-        <v>116</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>189</v>
-      </c>
-      <c r="B82" t="s">
-        <v>190</v>
-      </c>
-      <c r="C82" t="s">
-        <v>191</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>184</v>
-      </c>
-      <c r="B83" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>55</v>
-      </c>
-      <c r="B84" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>117</v>
-      </c>
-      <c r="B85" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>119</v>
-      </c>
-      <c r="B86" t="s">
-        <v>120</v>
-      </c>
-      <c r="C86" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>208</v>
-      </c>
-      <c r="B87" t="s">
-        <v>209</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>32</v>
-      </c>
-      <c r="B88" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>59</v>
-      </c>
-      <c r="B89" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>162</v>
-      </c>
-      <c r="B90" t="s">
-        <v>163</v>
-      </c>
-      <c r="C90" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>121</v>
-      </c>
-      <c r="B91" t="s">
-        <v>122</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>123</v>
-      </c>
-      <c r="B92" t="s">
-        <v>124</v>
-      </c>
-      <c r="C92" t="s">
-        <v>125</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>176</v>
-      </c>
-      <c r="B93" t="s">
-        <v>177</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>126</v>
-      </c>
-      <c r="B94" t="s">
-        <v>127</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>128</v>
-      </c>
-      <c r="B95" t="s">
-        <v>129</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>183</v>
+      <c r="B98" t="s">
+        <v>222</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>223</v>
+      </c>
+      <c r="B99" t="s">
+        <v>224</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>227</v>
+      </c>
+      <c r="B100" t="s">
+        <v>228</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Kleine update + woordenlijst update
</commit_message>
<xml_diff>
--- a/DLP woordenlijst.xlsx
+++ b/DLP woordenlijst.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanp\Documents\Paradox Interactive\Crusader Kings III\mod\DLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463E1218-AD2D-4289-8E22-C54146F5BE3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C088A4E0-5599-46D7-A802-4856B5A5AC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="237">
   <si>
     <t>Engelse term</t>
   </si>
@@ -784,6 +784,30 @@
   </si>
   <si>
     <t>Royeren/Ontslaan</t>
+  </si>
+  <si>
+    <t>Petty King</t>
+  </si>
+  <si>
+    <t>Klein-Koning</t>
+  </si>
+  <si>
+    <t>2024-05-28</t>
+  </si>
+  <si>
+    <t>Edit: Heb ik vertaald naar Heldenmoed</t>
+  </si>
+  <si>
+    <t>Court Physician</t>
+  </si>
+  <si>
+    <t>Hofarts</t>
+  </si>
+  <si>
+    <t>Level of Faith</t>
+  </si>
+  <si>
+    <t>Niveau van Toewijding</t>
   </si>
 </sst>
 </file>
@@ -1140,10 +1164,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1880,6 +1904,9 @@
       <c r="B71" t="s">
         <v>40</v>
       </c>
+      <c r="E71" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
@@ -2201,6 +2228,50 @@
       </c>
       <c r="D100" s="1" t="s">
         <v>214</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>229</v>
+      </c>
+      <c r="B101" t="s">
+        <v>230</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>233</v>
+      </c>
+      <c r="B102" t="s">
+        <v>234</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>184</v>
+      </c>
+      <c r="B103" t="s">
+        <v>185</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>235</v>
+      </c>
+      <c r="B104" t="s">
+        <v>236</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nog een kleine update
</commit_message>
<xml_diff>
--- a/DLP woordenlijst.xlsx
+++ b/DLP woordenlijst.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanp\Documents\Paradox Interactive\Crusader Kings III\mod\DLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C088A4E0-5599-46D7-A802-4856B5A5AC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E231F89-8CFE-4834-8E1F-16695EE74F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="261">
   <si>
     <t>Engelse term</t>
   </si>
@@ -808,6 +808,78 @@
   </si>
   <si>
     <t>Niveau van Toewijding</t>
+  </si>
+  <si>
+    <t>Involved</t>
+  </si>
+  <si>
+    <t>Betrokken</t>
+  </si>
+  <si>
+    <t>Tour</t>
+  </si>
+  <si>
+    <t>Toer(nee)</t>
+  </si>
+  <si>
+    <t>Tournaments</t>
+  </si>
+  <si>
+    <t>Toernooien</t>
+  </si>
+  <si>
+    <t>Pilgrimage</t>
+  </si>
+  <si>
+    <t>Pelgrimstocht</t>
+  </si>
+  <si>
+    <t>Holy Site/Holy Sites</t>
+  </si>
+  <si>
+    <t>Heiligdom/Heiligdommen</t>
+  </si>
+  <si>
+    <t>Quit</t>
+  </si>
+  <si>
+    <t>Verlaat</t>
+  </si>
+  <si>
+    <t>Hangt af van de context</t>
+  </si>
+  <si>
+    <t>Activity Guests</t>
+  </si>
+  <si>
+    <t>Activiteitenbezoekers</t>
+  </si>
+  <si>
+    <t>In dit specifieke geval liefst zo vertalen</t>
+  </si>
+  <si>
+    <t>Usurp</t>
+  </si>
+  <si>
+    <t>Inlijven</t>
+  </si>
+  <si>
+    <t>Revoked</t>
+  </si>
+  <si>
+    <t>Herroepen</t>
+  </si>
+  <si>
+    <t>Swear Fealty</t>
+  </si>
+  <si>
+    <t>Trouw Zweren</t>
+  </si>
+  <si>
+    <t>Faith</t>
+  </si>
+  <si>
+    <t>Godsdienst</t>
   </si>
 </sst>
 </file>
@@ -1164,10 +1236,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E104"/>
+  <dimension ref="A1:E115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="D111" sqref="D111:D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2274,6 +2346,133 @@
         <v>231</v>
       </c>
     </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>237</v>
+      </c>
+      <c r="B105" t="s">
+        <v>238</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>239</v>
+      </c>
+      <c r="B106" t="s">
+        <v>240</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>241</v>
+      </c>
+      <c r="B107" t="s">
+        <v>242</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>243</v>
+      </c>
+      <c r="B108" t="s">
+        <v>244</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>245</v>
+      </c>
+      <c r="B109" t="s">
+        <v>246</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>247</v>
+      </c>
+      <c r="B110" t="s">
+        <v>248</v>
+      </c>
+      <c r="C110" t="s">
+        <v>249</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>250</v>
+      </c>
+      <c r="B111" t="s">
+        <v>251</v>
+      </c>
+      <c r="C111" t="s">
+        <v>252</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>253</v>
+      </c>
+      <c r="B112" t="s">
+        <v>254</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>255</v>
+      </c>
+      <c r="B113" t="s">
+        <v>256</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>257</v>
+      </c>
+      <c r="B114" t="s">
+        <v>258</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>259</v>
+      </c>
+      <c r="B115" t="s">
+        <v>260</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Wat vertalingen erdoorheen gejast
</commit_message>
<xml_diff>
--- a/DLP woordenlijst.xlsx
+++ b/DLP woordenlijst.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanp\Documents\Paradox Interactive\Crusader Kings III\mod\DLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F45C86-DE6D-4D1C-8161-1AD5BA592813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5A0969-BB46-4A0C-8097-D139CBDB8BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31320" yWindow="2400" windowWidth="17595" windowHeight="17430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="304">
   <si>
     <t>Engelse term</t>
   </si>
@@ -979,6 +979,36 @@
   </si>
   <si>
     <t>Opstandige groep / Factie</t>
+  </si>
+  <si>
+    <t>Alliance</t>
+  </si>
+  <si>
+    <t>Bondgenootschap</t>
+  </si>
+  <si>
+    <t>Allies</t>
+  </si>
+  <si>
+    <t>Bondgenoten</t>
+  </si>
+  <si>
+    <t>Allied</t>
+  </si>
+  <si>
+    <t>Verbonden</t>
+  </si>
+  <si>
+    <t>Concubine</t>
+  </si>
+  <si>
+    <t>Bijvrouw</t>
+  </si>
+  <si>
+    <t>Heb zelf de context hiervan ietwat aangepast. Gezien het de Baanderheren waren die moesten worden opgeroepen en zij kwamen dan met de Heervaarders</t>
+  </si>
+  <si>
+    <t>Kolom1</t>
   </si>
 </sst>
 </file>
@@ -1034,13 +1064,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1064,17 +1093,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{620CAB14-0AE3-4DC1-ABD7-5524AAC7191E}" name="Tabel1" displayName="Tabel1" ref="A1:E151" totalsRowShown="0">
-  <autoFilter ref="A1:E151" xr:uid="{620CAB14-0AE3-4DC1-ABD7-5524AAC7191E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{620CAB14-0AE3-4DC1-ABD7-5524AAC7191E}" name="Tabel1" displayName="Tabel1" ref="A1:F151" totalsRowShown="0">
+  <autoFilter ref="A1:F151" xr:uid="{620CAB14-0AE3-4DC1-ABD7-5524AAC7191E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E123">
     <sortCondition ref="A1:A151"/>
   </sortState>
-  <tableColumns count="5">
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{BEFD245A-2A28-400B-A9E5-FE2EBA62AFD7}" name="Engelse term"/>
     <tableColumn id="2" xr3:uid="{C7771ADF-0301-48C6-AC98-3DC03BE980CB}" name="Nederlandse term"/>
     <tableColumn id="3" xr3:uid="{A302C31A-3B76-40AD-A403-4361CBAE6E9E}" name="uitleg"/>
     <tableColumn id="4" xr3:uid="{CBD3F489-A211-4D84-9CF0-2CB3C4563807}" name="Toegevoegd" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{39B66416-6FFC-4032-B8EE-7E2ABF7441BF}" name="Kolom"/>
+    <tableColumn id="6" xr3:uid="{25B7B3D6-5C40-4EAD-9C08-67B62FA7B971}" name="Kolom1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1343,10 +1373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E123"/>
+  <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="E124" sqref="E124"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F93" sqref="F93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,7 +1387,7 @@
     <col min="4" max="4" width="13.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1373,8 +1403,11 @@
       <c r="E1" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -1385,7 +1418,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>238</v>
       </c>
@@ -1399,7 +1432,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -1413,7 +1446,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1421,7 +1454,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>159</v>
       </c>
@@ -1429,7 +1462,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -1443,7 +1476,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>71</v>
       </c>
@@ -1454,7 +1487,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1462,7 +1495,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>135</v>
       </c>
@@ -1473,7 +1506,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -1487,7 +1520,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>201</v>
       </c>
@@ -1498,7 +1531,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -1506,7 +1539,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>166</v>
       </c>
@@ -1517,7 +1550,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>196</v>
       </c>
@@ -1531,7 +1564,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>139</v>
       </c>
@@ -2203,12 +2236,11 @@
       <c r="B80" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="C80" s="3"/>
       <c r="D80" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>227</v>
       </c>
@@ -2219,7 +2251,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>180</v>
       </c>
@@ -2233,7 +2265,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>101</v>
       </c>
@@ -2247,7 +2279,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>234</v>
       </c>
@@ -2258,7 +2290,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>20</v>
       </c>
@@ -2266,7 +2298,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>165</v>
       </c>
@@ -2277,7 +2309,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>64</v>
       </c>
@@ -2285,7 +2317,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>39</v>
       </c>
@@ -2299,7 +2331,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>134</v>
       </c>
@@ -2310,7 +2342,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>237</v>
       </c>
@@ -2324,7 +2356,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>104</v>
       </c>
@@ -2338,7 +2370,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>264</v>
       </c>
@@ -2351,8 +2383,11 @@
       <c r="E92" s="2" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F92" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>42</v>
       </c>
@@ -2363,7 +2398,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>66</v>
       </c>
@@ -2371,7 +2406,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>106</v>
       </c>
@@ -2382,7 +2417,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>108</v>
       </c>
@@ -2709,6 +2744,50 @@
       </c>
       <c r="D123" s="1" t="s">
         <v>177</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>294</v>
+      </c>
+      <c r="B124" t="s">
+        <v>295</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>296</v>
+      </c>
+      <c r="B125" t="s">
+        <v>297</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>298</v>
+      </c>
+      <c r="B126" t="s">
+        <v>299</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>300</v>
+      </c>
+      <c r="B127" t="s">
+        <v>301</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>